<commit_message>
for marius L ruh
</commit_message>
<xml_diff>
--- a/pav_3g_results_element.xlsx
+++ b/pav_3g_results_element.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,11 @@
           <t>J (in^4)</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Buckle ratio</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -488,7 +493,7 @@
         <v>13.3293328219011</v>
       </c>
       <c r="C2" t="n">
-        <v>350.8085118753277</v>
+        <v>337.2695627276308</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -497,10 +502,10 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>182.037715032449</v>
+        <v>175.0122316608695</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>-4.293176737148315e-11</v>
       </c>
       <c r="H2" t="n">
         <v>11.13329964228579</v>
@@ -510,6 +515,9 @@
       </c>
       <c r="J2" t="n">
         <v>30.50875810084839</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.9503561321756911</v>
       </c>
     </row>
     <row r="3">
@@ -520,7 +528,7 @@
         <v>11.92620796388136</v>
       </c>
       <c r="C3" t="n">
-        <v>648.5884725472937</v>
+        <v>625.8612525617799</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -529,10 +537,10 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>411.5262231595948</v>
+        <v>397.1059129020874</v>
       </c>
       <c r="G3" t="n">
-        <v>255.4719112730237</v>
+        <v>245.6123408854625</v>
       </c>
       <c r="H3" t="n">
         <v>15.03542838536893</v>
@@ -542,6 +550,9 @@
       </c>
       <c r="J3" t="n">
         <v>41.1933243942569</v>
+      </c>
+      <c r="K3" t="n">
+        <v>4.047704900001258</v>
       </c>
     </row>
     <row r="4">
@@ -552,7 +563,7 @@
         <v>10.5230984612139</v>
       </c>
       <c r="C4" t="n">
-        <v>851.6503690470763</v>
+        <v>822.9134908162224</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -561,10 +572,10 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>670.9809094673507</v>
+        <v>648.3402844041186</v>
       </c>
       <c r="G4" t="n">
-        <v>832.6369859218923</v>
+        <v>802.5533206764782</v>
       </c>
       <c r="H4" t="n">
         <v>20.85700578759742</v>
@@ -574,6 +585,9 @@
       </c>
       <c r="J4" t="n">
         <v>57.13138917018539</v>
+      </c>
+      <c r="K4" t="n">
+        <v>9.704344860264268</v>
       </c>
     </row>
     <row r="5">
@@ -584,7 +598,7 @@
         <v>9.11998902430812</v>
       </c>
       <c r="C5" t="n">
-        <v>929.8737230997223</v>
+        <v>897.9960599335344</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -593,10 +607,10 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>929.6332025122852</v>
+        <v>897.7637848035575</v>
       </c>
       <c r="G5" t="n">
-        <v>1776.266995095569</v>
+        <v>1714.34337620186</v>
       </c>
       <c r="H5" t="n">
         <v>29.81908969989933</v>
@@ -606,6 +620,9 @@
       </c>
       <c r="J5" t="n">
         <v>81.66401868197437</v>
+      </c>
+      <c r="K5" t="n">
+        <v>18.04893093899456</v>
       </c>
     </row>
     <row r="6">
@@ -616,7 +633,7 @@
         <v>7.716897869149379</v>
       </c>
       <c r="C6" t="n">
-        <v>960.7616251712776</v>
+        <v>926.9347789619342</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -625,10 +642,10 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>1199.174941515971</v>
+        <v>1156.953952186281</v>
       </c>
       <c r="G6" t="n">
-        <v>3085.117816057135</v>
+        <v>2978.324550276093</v>
       </c>
       <c r="H6" t="n">
         <v>41.56038618177409</v>
@@ -638,6 +655,9 @@
       </c>
       <c r="J6" t="n">
         <v>113.8005263867832</v>
+      </c>
+      <c r="K6" t="n">
+        <v>29.11339035925919</v>
       </c>
     </row>
     <row r="7">
@@ -648,7 +668,7 @@
         <v>6.31380669755022</v>
       </c>
       <c r="C7" t="n">
-        <v>970.7694476515321</v>
+        <v>935.5258614047922</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -657,10 +677,10 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>1479.545742326346</v>
+        <v>1425.831136760593</v>
       </c>
       <c r="G7" t="n">
-        <v>4773.462356519539</v>
+        <v>4607.22523950447</v>
       </c>
       <c r="H7" t="n">
         <v>56.03850053290055</v>
@@ -670,6 +690,9 @@
       </c>
       <c r="J7" t="n">
         <v>153.4238521439835</v>
+      </c>
+      <c r="K7" t="n">
+        <v>43.00304931844122</v>
       </c>
     </row>
     <row r="8">
@@ -680,7 +703,7 @@
         <v>4.91071552595106</v>
       </c>
       <c r="C8" t="n">
-        <v>967.2513896216407</v>
+        <v>930.9463650052438</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -689,10 +712,10 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>1767.727414800474</v>
+        <v>1701.377148470604</v>
       </c>
       <c r="G8" t="n">
-        <v>6856.547066284748</v>
+        <v>6614.683984933038</v>
       </c>
       <c r="H8" t="n">
         <v>73.54015248127043</v>
@@ -702,6 +725,9 @@
       </c>
       <c r="J8" t="n">
         <v>201.3179603616919</v>
+      </c>
+      <c r="K8" t="n">
+        <v>59.80142576705639</v>
       </c>
     </row>
     <row r="9">
@@ -712,7 +738,7 @@
         <v>3.541482800910612</v>
       </c>
       <c r="C9" t="n">
-        <v>907.8927243183883</v>
+        <v>872.831072611623</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -721,10 +747,10 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>2066.970959547968</v>
+        <v>1987.147194106904</v>
       </c>
       <c r="G9" t="n">
-        <v>9343.034846202201</v>
+        <v>9007.839350409757</v>
       </c>
       <c r="H9" t="n">
         <v>95.0524409160797</v>
@@ -734,6 +760,9 @@
       </c>
       <c r="J9" t="n">
         <v>260.4777634332362</v>
+      </c>
+      <c r="K9" t="n">
+        <v>79.43819985057675</v>
       </c>
     </row>
     <row r="10">
@@ -744,7 +773,7 @@
         <v>2.138443199620908</v>
       </c>
       <c r="C10" t="n">
-        <v>941.1124984146246</v>
+        <v>903.6782435342604</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -753,10 +782,10 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>2392.919650591456</v>
+        <v>2297.737444150311</v>
       </c>
       <c r="G10" t="n">
-        <v>12091.07281088431</v>
+        <v>11649.68579295559</v>
       </c>
       <c r="H10" t="n">
         <v>131.1626716055017</v>
@@ -766,6 +795,9 @@
       </c>
       <c r="J10" t="n">
         <v>359.352111215017</v>
+      </c>
+      <c r="K10" t="n">
+        <v>103.2178955249094</v>
       </c>
     </row>
     <row r="11">
@@ -776,7 +808,7 @@
         <v>0.7015453687862842</v>
       </c>
       <c r="C11" t="n">
-        <v>889.7643156612512</v>
+        <v>853.1687190743983</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -785,10 +817,10 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>2726.530229360825</v>
+        <v>2614.389296532579</v>
       </c>
       <c r="G11" t="n">
-        <v>15563.4261069627</v>
+        <v>14983.81667906232</v>
       </c>
       <c r="H11" t="n">
         <v>158.1238467263724</v>
@@ -798,6 +830,9 @@
       </c>
       <c r="J11" t="n">
         <v>432.6988362282643</v>
+      </c>
+      <c r="K11" t="n">
+        <v>131.5834403192706</v>
       </c>
     </row>
     <row r="12">
@@ -808,7 +843,7 @@
         <v>-0.7015452734313519</v>
       </c>
       <c r="C12" t="n">
-        <v>890.0183787210336</v>
+        <v>853.417191681895</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -817,10 +852,10 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>-2726.567508518727</v>
+        <v>-2614.439928077591</v>
       </c>
       <c r="G12" t="n">
-        <v>19383.21079244752</v>
+        <v>18646.69199201048</v>
       </c>
       <c r="H12" t="n">
         <v>158.0415340872649</v>
@@ -830,6 +865,9 @@
       </c>
       <c r="J12" t="n">
         <v>432.5107126974885</v>
+      </c>
+      <c r="K12" t="n">
+        <v>131.6411232115622</v>
       </c>
     </row>
     <row r="13">
@@ -840,7 +878,7 @@
         <v>-2.138400551527386</v>
       </c>
       <c r="C13" t="n">
-        <v>941.7175629512233</v>
+        <v>904.2670374911922</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -849,10 +887,10 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>-2393.134388611086</v>
+        <v>-2297.963454271599</v>
       </c>
       <c r="G13" t="n">
-        <v>15660.84178709845</v>
+        <v>15077.63455762345</v>
       </c>
       <c r="H13" t="n">
         <v>131.0098595088716</v>
@@ -862,6 +900,9 @@
       </c>
       <c r="J13" t="n">
         <v>359.002049802268</v>
+      </c>
+      <c r="K13" t="n">
+        <v>103.3026518664712</v>
       </c>
     </row>
     <row r="14">
@@ -872,7 +913,7 @@
         <v>-3.541419204433926</v>
       </c>
       <c r="C14" t="n">
-        <v>908.6368286230301</v>
+        <v>873.5564153245804</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -881,10 +922,10 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>-2067.325673701843</v>
+        <v>-1987.510904179655</v>
       </c>
       <c r="G14" t="n">
-        <v>12121.14035973588</v>
+        <v>11678.79904100214</v>
       </c>
       <c r="H14" t="n">
         <v>94.9405338476687</v>
@@ -894,6 +935,9 @@
       </c>
       <c r="J14" t="n">
         <v>260.221311185631</v>
+      </c>
+      <c r="K14" t="n">
+        <v>79.50517434511474</v>
       </c>
     </row>
     <row r="15">
@@ -904,7 +948,7 @@
         <v>-4.91067343847586</v>
       </c>
       <c r="C15" t="n">
-        <v>967.9365133135456</v>
+        <v>931.6159064490627</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
@@ -913,10 +957,10 @@
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>-1768.01965648942</v>
+        <v>-1701.676930506061</v>
       </c>
       <c r="G15" t="n">
-        <v>9347.258962057407</v>
+        <v>9012.017504124104</v>
       </c>
       <c r="H15" t="n">
         <v>73.46382858579754</v>
@@ -926,6 +970,9 @@
       </c>
       <c r="J15" t="n">
         <v>201.143415819404</v>
+      </c>
+      <c r="K15" t="n">
+        <v>59.84782283564201</v>
       </c>
     </row>
     <row r="16">
@@ -936,7 +983,7 @@
         <v>-6.31376461007502</v>
       </c>
       <c r="C16" t="n">
-        <v>971.4946565328453</v>
+        <v>936.2359146908516</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
@@ -945,10 +992,10 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>-1479.847215689575</v>
+        <v>-1426.13868462064</v>
       </c>
       <c r="G16" t="n">
-        <v>6858.025877452633</v>
+        <v>6616.189777222519</v>
       </c>
       <c r="H16" t="n">
         <v>55.98033776640718</v>
@@ -958,6 +1005,9 @@
       </c>
       <c r="J16" t="n">
         <v>153.2908183332579</v>
+      </c>
+      <c r="K16" t="n">
+        <v>43.0368592634219</v>
       </c>
     </row>
     <row r="17">
@@ -968,7 +1018,7 @@
         <v>-7.716855781674179</v>
       </c>
       <c r="C17" t="n">
-        <v>961.4811167631719</v>
+        <v>927.6396865498834</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
@@ -977,10 +1027,10 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>-1199.421091745652</v>
+        <v>-1157.204843849535</v>
       </c>
       <c r="G17" t="n">
-        <v>4774.51700020104</v>
+        <v>4608.298301605118</v>
       </c>
       <c r="H17" t="n">
         <v>41.51724765868896</v>
@@ -990,6 +1040,9 @@
       </c>
       <c r="J17" t="n">
         <v>113.7018374824549</v>
+      </c>
+      <c r="K17" t="n">
+        <v>29.13648317783106</v>
       </c>
     </row>
     <row r="18">
@@ -1000,7 +1053,7 @@
         <v>-9.119946936832919</v>
       </c>
       <c r="C18" t="n">
-        <v>930.5839165761951</v>
+        <v>898.692459366369</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -1009,10 +1062,10 @@
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>-929.8374807297741</v>
+        <v>-897.9716041541654</v>
       </c>
       <c r="G18" t="n">
-        <v>3085.826124191252</v>
+        <v>2979.044593352113</v>
       </c>
       <c r="H18" t="n">
         <v>29.78813594098335</v>
@@ -1022,6 +1075,9 @@
       </c>
       <c r="J18" t="n">
         <v>81.59318781441304</v>
+      </c>
+      <c r="K18" t="n">
+        <v>18.06340638119294</v>
       </c>
     </row>
     <row r="19">
@@ -1032,7 +1088,7 @@
         <v>-10.5230637719277</v>
       </c>
       <c r="C19" t="n">
-        <v>852.2974222769465</v>
+        <v>823.5477617982294</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
@@ -1041,10 +1097,10 @@
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>-671.1175692423658</v>
+        <v>-648.4794598773691</v>
       </c>
       <c r="G19" t="n">
-        <v>1776.954042932195</v>
+        <v>1715.027634685571</v>
       </c>
       <c r="H19" t="n">
         <v>20.83530823042767</v>
@@ -1054,6 +1110,9 @@
       </c>
       <c r="J19" t="n">
         <v>57.08172400600177</v>
+      </c>
+      <c r="K19" t="n">
+        <v>9.712277375218621</v>
       </c>
     </row>
     <row r="20">
@@ -1064,7 +1123,7 @@
         <v>-11.92618068922458</v>
       </c>
       <c r="C20" t="n">
-        <v>649.1141015709489</v>
+        <v>626.3769706185507</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -1073,10 +1132,10 @@
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>-411.6343630552467</v>
+        <v>-397.215658555278</v>
       </c>
       <c r="G20" t="n">
-        <v>833.1996293982207</v>
+        <v>803.1070853604114</v>
       </c>
       <c r="H20" t="n">
         <v>15.01974570569714</v>
@@ -1086,6 +1145,9 @@
       </c>
       <c r="J20" t="n">
         <v>41.15741590687573</v>
+      </c>
+      <c r="K20" t="n">
+        <v>4.051097989488993</v>
       </c>
     </row>
     <row r="21">
@@ -1096,7 +1158,7 @@
         <v>-13.32927197590668</v>
       </c>
       <c r="C21" t="n">
-        <v>351.0924747488394</v>
+        <v>337.5478961335763</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -1105,10 +1167,10 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>-182.0943838623993</v>
+        <v>-175.0694776767505</v>
       </c>
       <c r="G21" t="n">
-        <v>255.5392008195226</v>
+        <v>245.6809126371058</v>
       </c>
       <c r="H21" t="n">
         <v>11.12174078320303</v>
@@ -1118,6 +1180,9 @@
       </c>
       <c r="J21" t="n">
         <v>30.48226737205935</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.9511505493973414</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a wasted evening adding ttop/tbot for mruh
</commit_message>
<xml_diff>
--- a/pav_3g_results_element.xlsx
+++ b/pav_3g_results_element.xlsx
@@ -493,7 +493,7 @@
         <v>13.3293328219011</v>
       </c>
       <c r="C2" t="n">
-        <v>337.2695627275129</v>
+        <v>337.2695627278077</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -502,10 +502,10 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>175.0122316608172</v>
+        <v>175.0122316609742</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>-8.58635347429663e-11</v>
       </c>
       <c r="H2" t="n">
         <v>11.13329964228579</v>
@@ -517,7 +517,7 @@
         <v>30.50875810084839</v>
       </c>
       <c r="K2" t="n">
-        <v>0.4525505391311233</v>
+        <v>-0.4525505391315189</v>
       </c>
     </row>
     <row r="3">
@@ -528,7 +528,7 @@
         <v>11.92620796388136</v>
       </c>
       <c r="C3" t="n">
-        <v>625.8612525614425</v>
+        <v>625.8612525615872</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -537,10 +537,10 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>397.1059129017733</v>
+        <v>397.1059129019827</v>
       </c>
       <c r="G3" t="n">
-        <v>245.6123408853767</v>
+        <v>245.6123408855054</v>
       </c>
       <c r="H3" t="n">
         <v>15.03542838536893</v>
@@ -552,7 +552,7 @@
         <v>41.1933243942569</v>
       </c>
       <c r="K3" t="n">
-        <v>1.927478523809255</v>
+        <v>-1.024511054103239</v>
       </c>
     </row>
     <row r="4">
@@ -563,7 +563,7 @@
         <v>10.5230984612139</v>
       </c>
       <c r="C4" t="n">
-        <v>822.913490816106</v>
+        <v>822.9134908163769</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -572,10 +572,10 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>648.3402844040139</v>
+        <v>648.3402844044327</v>
       </c>
       <c r="G4" t="n">
-        <v>802.553320676006</v>
+        <v>802.5533206762635</v>
       </c>
       <c r="H4" t="n">
         <v>20.85700578759742</v>
@@ -587,7 +587,7 @@
         <v>57.13138917018539</v>
       </c>
       <c r="K4" t="n">
-        <v>4.621116600123874</v>
+        <v>-1.673079553805425</v>
       </c>
     </row>
     <row r="5">
@@ -598,7 +598,7 @@
         <v>9.11998902430812</v>
       </c>
       <c r="C5" t="n">
-        <v>897.9960599331073</v>
+        <v>897.9960599337786</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -607,10 +607,10 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>897.7637848030341</v>
+        <v>897.763784803767</v>
       </c>
       <c r="G5" t="n">
-        <v>1714.343376201173</v>
+        <v>1714.343376201689</v>
       </c>
       <c r="H5" t="n">
         <v>29.81908969989933</v>
@@ -622,7 +622,7 @@
         <v>81.66401868197437</v>
       </c>
       <c r="K5" t="n">
-        <v>8.59472901856522</v>
+        <v>-2.313735200304391</v>
       </c>
     </row>
     <row r="6">
@@ -633,7 +633,7 @@
         <v>7.716897869149379</v>
       </c>
       <c r="C6" t="n">
-        <v>926.9347789616651</v>
+        <v>926.9347789622033</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -642,10 +642,10 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>1156.953952185862</v>
+        <v>1156.953952186595</v>
       </c>
       <c r="G6" t="n">
-        <v>2978.324550274719</v>
+        <v>2978.324550276093</v>
       </c>
       <c r="H6" t="n">
         <v>41.56038618177409</v>
@@ -657,7 +657,7 @@
         <v>113.8005263867832</v>
       </c>
       <c r="K6" t="n">
-        <v>13.86351921868897</v>
+        <v>-2.976464721003201</v>
       </c>
     </row>
     <row r="7">
@@ -668,7 +668,7 @@
         <v>6.31380669755022</v>
       </c>
       <c r="C7" t="n">
-        <v>935.5258614047722</v>
+        <v>935.5258614050725</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -677,10 +677,10 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>1425.831136760593</v>
+        <v>1425.831136761117</v>
       </c>
       <c r="G7" t="n">
-        <v>4607.225239502581</v>
+        <v>4607.225239504814</v>
       </c>
       <c r="H7" t="n">
         <v>56.03850053290055</v>
@@ -692,7 +692,7 @@
         <v>153.4238521439835</v>
       </c>
       <c r="K7" t="n">
-        <v>20.47764253258408</v>
+        <v>-3.662948383454637</v>
       </c>
     </row>
     <row r="8">
@@ -703,7 +703,7 @@
         <v>4.91071552595106</v>
       </c>
       <c r="C8" t="n">
-        <v>930.9463650052941</v>
+        <v>930.9463650054442</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -712,10 +712,10 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>1701.377148470709</v>
+        <v>1701.377148470918</v>
       </c>
       <c r="G8" t="n">
-        <v>6614.683984931149</v>
+        <v>6614.683984933854</v>
       </c>
       <c r="H8" t="n">
         <v>73.54015248127043</v>
@@ -727,7 +727,7 @@
         <v>201.3179603616919</v>
       </c>
       <c r="K8" t="n">
-        <v>28.47686941287734</v>
+        <v>-4.365648273418756</v>
       </c>
     </row>
     <row r="9">
@@ -738,7 +738,7 @@
         <v>3.541482800910612</v>
       </c>
       <c r="C9" t="n">
-        <v>872.8310726117072</v>
+        <v>872.8310726118056</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -747,10 +747,10 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>1987.147194107166</v>
+        <v>1987.147194107323</v>
       </c>
       <c r="G9" t="n">
-        <v>9007.839350408081</v>
+        <v>9007.839350411174</v>
       </c>
       <c r="H9" t="n">
         <v>95.0524409160797</v>
@@ -762,7 +762,7 @@
         <v>260.4777634332362</v>
       </c>
       <c r="K9" t="n">
-        <v>37.82771421455472</v>
+        <v>-4.876124632317584</v>
       </c>
     </row>
     <row r="10">
@@ -773,7 +773,7 @@
         <v>2.138443199620908</v>
       </c>
       <c r="C10" t="n">
-        <v>903.6782435344323</v>
+        <v>903.6782435345085</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -782,10 +782,10 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>2297.73744415073</v>
+        <v>2297.737444150939</v>
       </c>
       <c r="G10" t="n">
-        <v>11649.68579295419</v>
+        <v>11649.68579295754</v>
       </c>
       <c r="H10" t="n">
         <v>131.1626716055017</v>
@@ -797,7 +797,7 @@
         <v>359.352111215017</v>
       </c>
       <c r="K10" t="n">
-        <v>49.15137882138144</v>
+        <v>-6.249526756895477</v>
       </c>
     </row>
     <row r="11">
@@ -808,7 +808,7 @@
         <v>0.7015453687862842</v>
       </c>
       <c r="C11" t="n">
-        <v>853.1687190745215</v>
+        <v>853.1687190745885</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -817,10 +817,10 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>2614.389296532946</v>
+        <v>2614.389296533142</v>
       </c>
       <c r="G11" t="n">
-        <v>14983.81667906162</v>
+        <v>14983.8166790652</v>
       </c>
       <c r="H11" t="n">
         <v>158.1238467263724</v>
@@ -832,7 +832,7 @@
         <v>432.6988362282643</v>
       </c>
       <c r="K11" t="n">
-        <v>62.65878110441299</v>
+        <v>-6.64920211999027</v>
       </c>
     </row>
     <row r="12">
@@ -843,7 +843,7 @@
         <v>-0.7015452734313519</v>
       </c>
       <c r="C12" t="n">
-        <v>853.4171916819231</v>
+        <v>853.4171916819225</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -852,10 +852,10 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>-2614.439928077669</v>
+        <v>-2614.439928077682</v>
       </c>
       <c r="G12" t="n">
-        <v>18646.69199200984</v>
+        <v>18646.69199200964</v>
       </c>
       <c r="H12" t="n">
         <v>158.0415340872649</v>
@@ -867,7 +867,7 @@
         <v>432.5107126974885</v>
       </c>
       <c r="K12" t="n">
-        <v>62.6862491483604</v>
+        <v>6.651181569588934</v>
       </c>
     </row>
     <row r="13">
@@ -878,7 +878,7 @@
         <v>-2.138400551527386</v>
       </c>
       <c r="C13" t="n">
-        <v>904.2670374912317</v>
+        <v>904.2670374912242</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -890,7 +890,7 @@
         <v>-2297.963454271704</v>
       </c>
       <c r="G13" t="n">
-        <v>15077.63455762272</v>
+        <v>15077.63455762254</v>
       </c>
       <c r="H13" t="n">
         <v>131.0098595088716</v>
@@ -902,7 +902,7 @@
         <v>359.002049802268</v>
       </c>
       <c r="K13" t="n">
-        <v>49.19173898403093</v>
+        <v>6.25367608101158</v>
       </c>
     </row>
     <row r="14">
@@ -913,7 +913,7 @@
         <v>-3.541419204433926</v>
       </c>
       <c r="C14" t="n">
-        <v>873.5564153246366</v>
+        <v>873.5564153245809</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -922,10 +922,10 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>-1987.510904179759</v>
+        <v>-1987.510904179602</v>
       </c>
       <c r="G14" t="n">
-        <v>11678.79904100141</v>
+        <v>11678.79904100106</v>
       </c>
       <c r="H14" t="n">
         <v>94.9405338476687</v>
@@ -937,7 +937,7 @@
         <v>260.221311185631</v>
       </c>
       <c r="K14" t="n">
-        <v>37.85960683100402</v>
+        <v>4.88023692952197</v>
       </c>
     </row>
     <row r="15">
@@ -948,7 +948,7 @@
         <v>-4.91067343847586</v>
       </c>
       <c r="C15" t="n">
-        <v>931.6159064490794</v>
+        <v>931.6159064490297</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
@@ -957,10 +957,10 @@
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>-1701.676930506061</v>
+        <v>-1701.676930506009</v>
       </c>
       <c r="G15" t="n">
-        <v>9012.017504123331</v>
+        <v>9012.017504123072</v>
       </c>
       <c r="H15" t="n">
         <v>73.46382858579754</v>
@@ -972,7 +972,7 @@
         <v>201.143415819404</v>
       </c>
       <c r="K15" t="n">
-        <v>28.49896325506473</v>
+        <v>4.368844526648956</v>
       </c>
     </row>
     <row r="16">
@@ -983,7 +983,7 @@
         <v>-6.31376461007502</v>
       </c>
       <c r="C16" t="n">
-        <v>936.2359146907116</v>
+        <v>936.2359146907713</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
@@ -992,10 +992,10 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>-1426.13868462043</v>
+        <v>-1426.138684620535</v>
       </c>
       <c r="G16" t="n">
-        <v>6616.189777221789</v>
+        <v>6616.189777221574</v>
       </c>
       <c r="H16" t="n">
         <v>55.98033776640718</v>
@@ -1007,7 +1007,7 @@
         <v>153.2908183332579</v>
       </c>
       <c r="K16" t="n">
-        <v>20.49374250638927</v>
+        <v>3.665775890114592</v>
       </c>
     </row>
     <row r="17">
@@ -1018,7 +1018,7 @@
         <v>-7.716855781674179</v>
       </c>
       <c r="C17" t="n">
-        <v>927.6396865499323</v>
+        <v>927.6396865495901</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
@@ -1027,10 +1027,10 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>-1157.204843849744</v>
+        <v>-1157.204843849326</v>
       </c>
       <c r="G17" t="n">
-        <v>4608.298301604603</v>
+        <v>4608.298301604259</v>
       </c>
       <c r="H17" t="n">
         <v>41.51724765868896</v>
@@ -1042,7 +1042,7 @@
         <v>113.7018374824549</v>
       </c>
       <c r="K17" t="n">
-        <v>13.87451579896513</v>
+        <v>2.978766731585818</v>
       </c>
     </row>
     <row r="18">
@@ -1053,7 +1053,7 @@
         <v>-9.119946936832919</v>
       </c>
       <c r="C18" t="n">
-        <v>898.6924593661862</v>
+        <v>898.6924593665523</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -1062,10 +1062,10 @@
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>-897.9716041540607</v>
+        <v>-897.9716041544795</v>
       </c>
       <c r="G18" t="n">
-        <v>2979.044593351512</v>
+        <v>2979.044593351941</v>
       </c>
       <c r="H18" t="n">
         <v>29.78813594098335</v>
@@ -1077,7 +1077,7 @@
         <v>81.59318781441304</v>
       </c>
       <c r="K18" t="n">
-        <v>8.601622086280626</v>
+        <v>2.31555943445677</v>
       </c>
     </row>
     <row r="19">
@@ -1088,7 +1088,7 @@
         <v>-10.5230637719277</v>
       </c>
       <c r="C19" t="n">
-        <v>823.5477617976479</v>
+        <v>823.5477617979968</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
@@ -1097,10 +1097,10 @@
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>-648.4794598768457</v>
+        <v>-648.4794598771598</v>
       </c>
       <c r="G19" t="n">
-        <v>1715.027634685142</v>
+        <v>1715.027634685314</v>
       </c>
       <c r="H19" t="n">
         <v>20.83530823042767</v>
@@ -1112,7 +1112,7 @@
         <v>57.08172400600177</v>
       </c>
       <c r="K19" t="n">
-        <v>4.62489398819895</v>
+        <v>1.674390738614533</v>
       </c>
     </row>
     <row r="20">
@@ -1123,7 +1123,7 @@
         <v>-11.92618068922458</v>
       </c>
       <c r="C20" t="n">
-        <v>626.3769706186472</v>
+        <v>626.3769706185988</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -1135,7 +1135,7 @@
         <v>-397.2156585554874</v>
       </c>
       <c r="G20" t="n">
-        <v>803.1070853604543</v>
+        <v>803.1070853603685</v>
       </c>
       <c r="H20" t="n">
         <v>15.01974570569714</v>
@@ -1147,7 +1147,7 @@
         <v>41.15741590687573</v>
       </c>
       <c r="K20" t="n">
-        <v>1.929094280709044</v>
+        <v>1.025368515122934</v>
       </c>
     </row>
     <row r="21">
@@ -1158,7 +1158,7 @@
         <v>-13.32927197590668</v>
       </c>
       <c r="C21" t="n">
-        <v>337.5478961336943</v>
+        <v>337.5478961334583</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -1167,10 +1167,10 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>-175.0694776767505</v>
+        <v>-175.0694776766458</v>
       </c>
       <c r="G21" t="n">
-        <v>245.6809126371058</v>
+        <v>245.6809126370629</v>
       </c>
       <c r="H21" t="n">
         <v>11.12174078320303</v>
@@ -1182,7 +1182,7 @@
         <v>30.48226737205935</v>
       </c>
       <c r="K21" t="n">
-        <v>0.4529288330465115</v>
+        <v>0.4529288330461948</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update new mass model
</commit_message>
<xml_diff>
--- a/pav_3g_results_element.xlsx
+++ b/pav_3g_results_element.xlsx
@@ -493,7 +493,7 @@
         <v>13.3293328219011</v>
       </c>
       <c r="C2" t="n">
-        <v>337.2695627276308</v>
+        <v>337.301872878912</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -502,10 +502,10 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>175.0122316608695</v>
+        <v>175.0122316609742</v>
       </c>
       <c r="G2" t="n">
-        <v>-4.293176737148315e-11</v>
+        <v>-8.58635347429663e-11</v>
       </c>
       <c r="H2" t="n">
         <v>11.13329964228579</v>
@@ -517,7 +517,7 @@
         <v>30.50875810084839</v>
       </c>
       <c r="K2" t="n">
-        <v>0.9503561321756911</v>
+        <v>0.4525505391315189</v>
       </c>
     </row>
     <row r="3">
@@ -528,7 +528,7 @@
         <v>11.92620796388136</v>
       </c>
       <c r="C3" t="n">
-        <v>625.8612525617799</v>
+        <v>1177.61873778985</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -537,10 +537,10 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>397.1059129020874</v>
+        <v>397.1059129019827</v>
       </c>
       <c r="G3" t="n">
-        <v>245.6123408854625</v>
+        <v>245.6123408855054</v>
       </c>
       <c r="H3" t="n">
         <v>15.03542838536893</v>
@@ -552,7 +552,7 @@
         <v>41.1933243942569</v>
       </c>
       <c r="K3" t="n">
-        <v>4.047704900001258</v>
+        <v>1.92747852380969</v>
       </c>
     </row>
     <row r="4">
@@ -563,7 +563,7 @@
         <v>10.5230984612139</v>
       </c>
       <c r="C4" t="n">
-        <v>822.9134908162224</v>
+        <v>2271.270931647058</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -572,10 +572,10 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>648.3402844041186</v>
+        <v>648.3402844044327</v>
       </c>
       <c r="G4" t="n">
-        <v>802.5533206764782</v>
+        <v>802.5533206762635</v>
       </c>
       <c r="H4" t="n">
         <v>20.85700578759742</v>
@@ -587,7 +587,7 @@
         <v>57.13138917018539</v>
       </c>
       <c r="K4" t="n">
-        <v>9.704344860264268</v>
+        <v>4.617308479895989</v>
       </c>
     </row>
     <row r="5">
@@ -598,7 +598,7 @@
         <v>9.11998902430812</v>
       </c>
       <c r="C5" t="n">
-        <v>897.9960599335344</v>
+        <v>3334.050946095882</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -607,10 +607,10 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>897.7637848035575</v>
+        <v>897.763784803767</v>
       </c>
       <c r="G5" t="n">
-        <v>1714.34337620186</v>
+        <v>1714.343376201689</v>
       </c>
       <c r="H5" t="n">
         <v>29.81908969989933</v>
@@ -622,7 +622,7 @@
         <v>81.66401868197437</v>
       </c>
       <c r="K5" t="n">
-        <v>18.04893093899456</v>
+        <v>8.589657843470457</v>
       </c>
     </row>
     <row r="6">
@@ -633,7 +633,7 @@
         <v>7.716897869149379</v>
       </c>
       <c r="C6" t="n">
-        <v>926.9347789619342</v>
+        <v>4316.75863830004</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -642,7 +642,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>1156.953952186281</v>
+        <v>1156.953952186595</v>
       </c>
       <c r="G6" t="n">
         <v>2978.324550276093</v>
@@ -657,7 +657,7 @@
         <v>113.8005263867832</v>
       </c>
       <c r="K6" t="n">
-        <v>29.11339035925919</v>
+        <v>13.86047259264091</v>
       </c>
     </row>
     <row r="7">
@@ -668,7 +668,7 @@
         <v>6.31380669755022</v>
       </c>
       <c r="C7" t="n">
-        <v>935.5258614047922</v>
+        <v>5229.865727713754</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -677,10 +677,10 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>1425.831136760593</v>
+        <v>1425.831136761117</v>
       </c>
       <c r="G7" t="n">
-        <v>4607.22523950447</v>
+        <v>4607.225239504814</v>
       </c>
       <c r="H7" t="n">
         <v>56.03850053290055</v>
@@ -692,7 +692,7 @@
         <v>153.4238521439835</v>
       </c>
       <c r="K7" t="n">
-        <v>43.00304931844122</v>
+        <v>20.47561536281522</v>
       </c>
     </row>
     <row r="8">
@@ -703,7 +703,7 @@
         <v>4.91071552595106</v>
       </c>
       <c r="C8" t="n">
-        <v>930.9463650052438</v>
+        <v>6072.574524034305</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -712,10 +712,10 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>1701.377148470604</v>
+        <v>1701.377148470918</v>
       </c>
       <c r="G8" t="n">
-        <v>6614.683984933038</v>
+        <v>6614.683984933854</v>
       </c>
       <c r="H8" t="n">
         <v>73.54015248127043</v>
@@ -727,7 +727,7 @@
         <v>201.3179603616919</v>
       </c>
       <c r="K8" t="n">
-        <v>59.80142576705639</v>
+        <v>28.47542750499196</v>
       </c>
     </row>
     <row r="9">
@@ -738,7 +738,7 @@
         <v>3.541482800910612</v>
       </c>
       <c r="C9" t="n">
-        <v>872.831072611623</v>
+        <v>6765.849125159718</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -747,10 +747,10 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>1987.147194106904</v>
+        <v>1987.147194107323</v>
       </c>
       <c r="G9" t="n">
-        <v>9007.839350409757</v>
+        <v>9007.839350411174</v>
       </c>
       <c r="H9" t="n">
         <v>95.0524409160797</v>
@@ -762,7 +762,7 @@
         <v>260.4777634332362</v>
       </c>
       <c r="K9" t="n">
-        <v>79.43819985057675</v>
+        <v>37.79535684183598</v>
       </c>
     </row>
     <row r="10">
@@ -773,7 +773,7 @@
         <v>2.138443199620908</v>
       </c>
       <c r="C10" t="n">
-        <v>903.6782435342604</v>
+        <v>7050.874324237787</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -782,10 +782,10 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>2297.737444150311</v>
+        <v>2297.737444150939</v>
       </c>
       <c r="G10" t="n">
-        <v>11649.68579295559</v>
+        <v>11649.68579295754</v>
       </c>
       <c r="H10" t="n">
         <v>131.1626716055017</v>
@@ -797,7 +797,7 @@
         <v>359.352111215017</v>
       </c>
       <c r="K10" t="n">
-        <v>103.2178955249094</v>
+        <v>48.7581256366926</v>
       </c>
     </row>
     <row r="11">
@@ -808,7 +808,7 @@
         <v>0.7015453687862842</v>
       </c>
       <c r="C11" t="n">
-        <v>853.1687190743983</v>
+        <v>7838.960082260692</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -817,10 +817,10 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>2614.389296532579</v>
+        <v>2614.389296533142</v>
       </c>
       <c r="G11" t="n">
-        <v>14983.81667906232</v>
+        <v>14983.8166790652</v>
       </c>
       <c r="H11" t="n">
         <v>158.1238467263724</v>
@@ -832,7 +832,7 @@
         <v>432.6988362282643</v>
       </c>
       <c r="K11" t="n">
-        <v>131.5834403192706</v>
+        <v>61.08817982711074</v>
       </c>
     </row>
     <row r="12">
@@ -843,7 +843,7 @@
         <v>-0.7015452734313519</v>
       </c>
       <c r="C12" t="n">
-        <v>853.417191681895</v>
+        <v>7842.34378029345</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -852,10 +852,10 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>-2614.439928077591</v>
+        <v>-2614.439928077682</v>
       </c>
       <c r="G12" t="n">
-        <v>18646.69199201048</v>
+        <v>18646.69199200964</v>
       </c>
       <c r="H12" t="n">
         <v>158.0415340872649</v>
@@ -867,7 +867,7 @@
         <v>432.5107126974885</v>
       </c>
       <c r="K12" t="n">
-        <v>131.6411232115622</v>
+        <v>61.11501429253024</v>
       </c>
     </row>
     <row r="13">
@@ -878,7 +878,7 @@
         <v>-2.138400551527386</v>
       </c>
       <c r="C13" t="n">
-        <v>904.2670374911922</v>
+        <v>7056.523220242473</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -887,10 +887,10 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>-2297.963454271599</v>
+        <v>-2297.963454271704</v>
       </c>
       <c r="G13" t="n">
-        <v>15077.63455762345</v>
+        <v>15077.63455762254</v>
       </c>
       <c r="H13" t="n">
         <v>131.0098595088716</v>
@@ -902,7 +902,7 @@
         <v>359.002049802268</v>
       </c>
       <c r="K13" t="n">
-        <v>103.3026518664712</v>
+        <v>48.79778864770837</v>
       </c>
     </row>
     <row r="14">
@@ -913,7 +913,7 @@
         <v>-3.541419204433926</v>
       </c>
       <c r="C14" t="n">
-        <v>873.5564153245804</v>
+        <v>6771.468230732743</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -922,10 +922,10 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>-1987.510904179655</v>
+        <v>-1987.510904179602</v>
       </c>
       <c r="G14" t="n">
-        <v>11678.79904100214</v>
+        <v>11678.79904100106</v>
       </c>
       <c r="H14" t="n">
         <v>94.9405338476687</v>
@@ -937,7 +937,7 @@
         <v>260.221311185631</v>
       </c>
       <c r="K14" t="n">
-        <v>79.50517434511474</v>
+        <v>37.82721141996331</v>
       </c>
     </row>
     <row r="15">
@@ -948,7 +948,7 @@
         <v>-4.91067343847586</v>
       </c>
       <c r="C15" t="n">
-        <v>931.6159064490627</v>
+        <v>6077.207375224643</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
@@ -957,10 +957,10 @@
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>-1701.676930506061</v>
+        <v>-1701.676930506009</v>
       </c>
       <c r="G15" t="n">
-        <v>9012.017504124104</v>
+        <v>9012.017504123072</v>
       </c>
       <c r="H15" t="n">
         <v>73.46382858579754</v>
@@ -972,7 +972,7 @@
         <v>201.143415819404</v>
       </c>
       <c r="K15" t="n">
-        <v>59.84782283564201</v>
+        <v>28.4975192406987</v>
       </c>
     </row>
     <row r="16">
@@ -983,7 +983,7 @@
         <v>-6.31376461007502</v>
       </c>
       <c r="C16" t="n">
-        <v>936.2359146908516</v>
+        <v>5233.909756217452</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
@@ -992,10 +992,10 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>-1426.13868462064</v>
+        <v>-1426.138684620535</v>
       </c>
       <c r="G16" t="n">
-        <v>6616.189777222519</v>
+        <v>6616.189777221574</v>
       </c>
       <c r="H16" t="n">
         <v>55.98033776640718</v>
@@ -1007,7 +1007,7 @@
         <v>153.2908183332579</v>
       </c>
       <c r="K16" t="n">
-        <v>43.0368592634219</v>
+        <v>20.49171240990674</v>
       </c>
     </row>
     <row r="17">
@@ -1018,7 +1018,7 @@
         <v>-7.716855781674179</v>
       </c>
       <c r="C17" t="n">
-        <v>927.6396865498834</v>
+        <v>4320.12641280349</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
@@ -1027,10 +1027,10 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>-1157.204843849535</v>
+        <v>-1157.204843849326</v>
       </c>
       <c r="G17" t="n">
-        <v>4608.298301605118</v>
+        <v>4608.298301604259</v>
       </c>
       <c r="H17" t="n">
         <v>41.51724765868896</v>
@@ -1042,7 +1042,7 @@
         <v>113.7018374824549</v>
       </c>
       <c r="K17" t="n">
-        <v>29.13648317783106</v>
+        <v>13.87146478033595</v>
       </c>
     </row>
     <row r="18">
@@ -1053,7 +1053,7 @@
         <v>-9.119946936832919</v>
       </c>
       <c r="C18" t="n">
-        <v>898.692459366369</v>
+        <v>3336.680672534461</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -1062,10 +1062,10 @@
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>-897.9716041541654</v>
+        <v>-897.9716041544795</v>
       </c>
       <c r="G18" t="n">
-        <v>2979.044593352113</v>
+        <v>2979.044593351941</v>
       </c>
       <c r="H18" t="n">
         <v>29.78813594098335</v>
@@ -1077,7 +1077,7 @@
         <v>81.59318781441304</v>
       </c>
       <c r="K18" t="n">
-        <v>18.06340638119294</v>
+        <v>8.596543661801414</v>
       </c>
     </row>
     <row r="19">
@@ -1088,7 +1088,7 @@
         <v>-10.5230637719277</v>
       </c>
       <c r="C19" t="n">
-        <v>823.5477617982294</v>
+        <v>2273.097302460856</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
@@ -1097,10 +1097,10 @@
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>-648.4794598773691</v>
+        <v>-648.4794598771598</v>
       </c>
       <c r="G19" t="n">
-        <v>1715.027634685571</v>
+        <v>1715.027634685314</v>
       </c>
       <c r="H19" t="n">
         <v>20.83530823042767</v>
@@ -1112,7 +1112,7 @@
         <v>57.08172400600177</v>
       </c>
       <c r="K19" t="n">
-        <v>9.712277375218621</v>
+        <v>4.621080887771636</v>
       </c>
     </row>
     <row r="20">
@@ -1123,7 +1123,7 @@
         <v>-11.92618068922458</v>
       </c>
       <c r="C20" t="n">
-        <v>626.3769706185507</v>
+        <v>1178.590700430782</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -1132,10 +1132,10 @@
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>-397.215658555278</v>
+        <v>-397.2156585554874</v>
       </c>
       <c r="G20" t="n">
-        <v>803.1070853604114</v>
+        <v>803.1070853603685</v>
       </c>
       <c r="H20" t="n">
         <v>15.01974570569714</v>
@@ -1147,7 +1147,7 @@
         <v>41.15741590687573</v>
       </c>
       <c r="K20" t="n">
-        <v>4.051097989488993</v>
+        <v>1.929094280708807</v>
       </c>
     </row>
     <row r="21">
@@ -1158,7 +1158,7 @@
         <v>-13.32927197590668</v>
       </c>
       <c r="C21" t="n">
-        <v>337.5478961335763</v>
+        <v>337.5814046661731</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -1167,10 +1167,10 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>-175.0694776767505</v>
+        <v>-175.0694776766458</v>
       </c>
       <c r="G21" t="n">
-        <v>245.6809126371058</v>
+        <v>245.6809126370629</v>
       </c>
       <c r="H21" t="n">
         <v>11.12174078320303</v>
@@ -1182,7 +1182,7 @@
         <v>30.48226737205935</v>
       </c>
       <c r="K21" t="n">
-        <v>0.9511505493973414</v>
+        <v>0.4529288330461948</v>
       </c>
     </row>
   </sheetData>

</xml_diff>